<commit_message>
add fritzing sketch and update shoulderjoint servomount
</commit_message>
<xml_diff>
--- a/electronics/SpotMicroESP32_Pinout_v1_1_0_with_ESP32_CAM.xlsx
+++ b/electronics/SpotMicroESP32_Pinout_v1_1_0_with_ESP32_CAM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kubin\Projekte\SpotMicroESP32\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C3DA49E-EC91-404B-AFCD-71875D4140EF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44DFB44-748B-4617-A368-6AA01AE0E1FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{F9FC6447-11F2-4062-BA4B-EAD886E6EF95}"/>
   </bookViews>
@@ -166,7 +166,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="89">
   <si>
     <t>3.3V</t>
   </si>
@@ -327,9 +327,6 @@
     <t>LED GND</t>
   </si>
   <si>
-    <t>POWERBUS</t>
-  </si>
-  <si>
     <t>GPIO12</t>
   </si>
   <si>
@@ -402,22 +399,40 @@
     <t>SD-CARD 1Bit Mode (SPI-MODE)</t>
   </si>
   <si>
-    <t>POWERBUS 3V3</t>
-  </si>
-  <si>
-    <t>POWERBUS 5V</t>
-  </si>
-  <si>
-    <t>POWERBUS I2C CLK</t>
-  </si>
-  <si>
-    <t>POWERBUS I2C DATA</t>
-  </si>
-  <si>
-    <t>adc</t>
-  </si>
-  <si>
-    <t>i2c2</t>
+    <t>TO POWERBUS 3V3</t>
+  </si>
+  <si>
+    <t>FROM POWERBUS 5V</t>
+  </si>
+  <si>
+    <t>TO POWERBUS I2C CLK</t>
+  </si>
+  <si>
+    <t>TO POWERBUS I2C DATA</t>
+  </si>
+  <si>
+    <t>VOLTAGE SENSOR</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>CURRENT SENSOR</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>PCA9685</t>
+  </si>
+  <si>
+    <t>I2C Clock</t>
+  </si>
+  <si>
+    <t>I2C Data</t>
+  </si>
+  <si>
+    <t>unassigned</t>
   </si>
 </sst>
 </file>
@@ -538,7 +553,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="26">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -668,12 +683,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -684,8 +693,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -863,15 +884,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
     <border diagonalUp="1" diagonalDown="1">
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color auto="1"/>
+      <top style="medium">
+        <color indexed="64"/>
       </top>
       <bottom/>
       <diagonal style="thin">
@@ -879,26 +920,11 @@
       </diagonal>
     </border>
     <border diagonalUp="1" diagonalDown="1">
-      <left style="thin">
-        <color auto="1"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal style="thin">
-        <color auto="1"/>
-      </diagonal>
-    </border>
-    <border diagonalUp="1" diagonalDown="1">
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
+      <right style="medium">
+        <color indexed="64"/>
       </right>
       <top/>
       <bottom/>
@@ -906,24 +932,28 @@
         <color auto="1"/>
       </diagonal>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+    <border diagonalUp="1" diagonalDown="1">
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
-      <diagonal/>
+      <diagonal style="thin">
+        <color auto="1"/>
+      </diagonal>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
@@ -933,34 +963,48 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left style="medium">
+        <color indexed="64"/>
       </left>
-      <right/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="medium">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -973,7 +1017,7 @@
     <xf numFmtId="0" fontId="12" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="93">
+  <cellXfs count="105">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
@@ -1030,7 +1074,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1060,54 +1103,17 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="23" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="13" xfId="6"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="14" xfId="5" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="18" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="19" xfId="5" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="18" xfId="6" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="20" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="17" borderId="12" xfId="6" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1132,9 +1138,75 @@
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="20" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="21" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="22" xfId="5" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="11" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="23" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="6" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Ausgabe" xfId="5" builtinId="21"/>
@@ -1245,7 +1317,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>3546528</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>57150</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1774,7 +1846,7 @@
   <dimension ref="D1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,11 +1864,11 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="4:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="77"/>
+      <c r="D3" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="67"/>
+      <c r="F3" s="68"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1804,14 +1876,14 @@
       <c r="I3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="78" t="s">
-        <v>78</v>
-      </c>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
+      <c r="J3" s="66" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="67"/>
+      <c r="L3" s="68"/>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F4" s="35"/>
+      <c r="F4" s="34"/>
       <c r="G4" s="8" t="s">
         <v>35</v>
       </c>
@@ -1819,13 +1891,16 @@
       <c r="I4" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="91"/>
-      <c r="K4" s="92"/>
-      <c r="L4" s="92"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="57"/>
+      <c r="L4" s="57"/>
     </row>
     <row r="5" spans="4:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="F5" t="s">
+      <c r="E5" s="73" t="s">
         <v>82</v>
+      </c>
+      <c r="F5" s="70" t="s">
+        <v>81</v>
       </c>
       <c r="G5" s="9" t="s">
         <v>2</v>
@@ -1834,19 +1909,22 @@
       <c r="I5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="82" t="s">
+      <c r="J5" s="58" t="s">
         <v>36</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="75" t="s">
-        <v>80</v>
+      <c r="L5" s="69" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F6" s="35" t="s">
-        <v>82</v>
+      <c r="E6" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="F6" s="71" t="s">
+        <v>83</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>3</v>
@@ -1855,14 +1933,14 @@
       <c r="I6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="83"/>
+      <c r="J6" s="59"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="43" t="s">
+      <c r="F7" s="42" t="s">
         <v>46</v>
       </c>
       <c r="G7" s="10" t="s">
@@ -1872,14 +1950,14 @@
       <c r="I7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="83"/>
+      <c r="J7" s="59"/>
       <c r="K7" s="31"/>
     </row>
     <row r="8" spans="4:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E8" s="44" t="s">
+      <c r="E8" s="43" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="45" t="s">
+      <c r="F8" s="44" t="s">
         <v>47</v>
       </c>
       <c r="G8" s="10" t="s">
@@ -1889,19 +1967,19 @@
       <c r="I8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="84"/>
+      <c r="J8" s="60"/>
       <c r="K8" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="75" t="s">
-        <v>81</v>
+      <c r="L8" s="69" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E9" s="44" t="s">
+      <c r="E9" s="43" t="s">
         <v>48</v>
       </c>
-      <c r="F9" s="45" t="s">
+      <c r="F9" s="44" t="s">
         <v>47</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -1911,18 +1989,18 @@
       <c r="I9" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="J9" s="46" t="s">
+      <c r="J9" s="45" t="s">
         <v>43</v>
       </c>
-      <c r="K9" s="47" t="s">
+      <c r="K9" s="46" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="10" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E10" s="42" t="s">
+      <c r="E10" s="41" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="43" t="s">
+      <c r="F10" s="42" t="s">
         <v>46</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -1932,16 +2010,19 @@
       <c r="I10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="90" t="s">
-        <v>83</v>
+      <c r="J10" s="77" t="s">
+        <v>85</v>
+      </c>
+      <c r="K10" s="79" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="11" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D11" s="23"/>
-      <c r="E11" s="40" t="s">
+      <c r="E11" s="39" t="s">
         <v>50</v>
       </c>
-      <c r="F11" s="41" t="s">
+      <c r="F11" s="40" t="s">
         <v>51</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -1951,8 +2032,9 @@
       <c r="I11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="90" t="s">
-        <v>83</v>
+      <c r="J11" s="78"/>
+      <c r="K11" s="79" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="12" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1965,13 +2047,13 @@
       <c r="I12" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="J12" s="90"/>
+      <c r="J12" s="55"/>
     </row>
     <row r="13" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="38" t="s">
+      <c r="E13" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F13" s="39" t="s">
+      <c r="F13" s="38" t="s">
         <v>44</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -1981,15 +2063,15 @@
       <c r="I13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="85" t="s">
+      <c r="J13" s="61" t="s">
         <v>41</v>
       </c>
-      <c r="K13" s="33" t="s">
+      <c r="K13" s="32" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="14" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F14" s="90"/>
+      <c r="F14" s="55"/>
       <c r="G14" s="11" t="s">
         <v>12</v>
       </c>
@@ -1997,13 +2079,13 @@
       <c r="I14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="86"/>
-      <c r="K14" s="34" t="s">
+      <c r="J14" s="62"/>
+      <c r="K14" s="33" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="15" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F15" s="90"/>
+      <c r="F15" s="55"/>
       <c r="G15" s="11" t="s">
         <v>11</v>
       </c>
@@ -2011,14 +2093,14 @@
       <c r="I15" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="90"/>
+      <c r="J15" s="55"/>
     </row>
     <row r="16" spans="4:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" s="80"/>
-      <c r="F16" s="81"/>
+      <c r="D16" s="74" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="75"/>
+      <c r="F16" s="76"/>
       <c r="G16" s="24" t="s">
         <v>1</v>
       </c>
@@ -2026,7 +2108,7 @@
       <c r="I16" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J16" s="90"/>
+      <c r="J16" s="55"/>
     </row>
     <row r="17" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="G17" s="25" t="s">
@@ -2036,15 +2118,15 @@
       <c r="I17" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="J17" s="36" t="s">
+      <c r="J17" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="K17" s="37" t="s">
+      <c r="K17" s="36" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="18" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F18" s="35"/>
+      <c r="F18" s="34"/>
       <c r="G18" s="12" t="s">
         <v>14</v>
       </c>
@@ -2054,7 +2136,7 @@
       </c>
     </row>
     <row r="19" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F19" s="35"/>
+      <c r="F19" s="34"/>
       <c r="G19" s="13" t="s">
         <v>15</v>
       </c>
@@ -2062,10 +2144,10 @@
       <c r="I19" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="J19" s="35"/>
+      <c r="J19" s="34"/>
     </row>
     <row r="20" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F20" s="35"/>
+      <c r="F20" s="34"/>
       <c r="G20" s="14" t="s">
         <v>16</v>
       </c>
@@ -2073,14 +2155,14 @@
       <c r="I20" s="19" t="s">
         <v>33</v>
       </c>
-      <c r="J20" s="35"/>
+      <c r="J20" s="34"/>
     </row>
     <row r="21" spans="4:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="80" t="s">
-        <v>79</v>
-      </c>
-      <c r="E21" s="80"/>
-      <c r="F21" s="81"/>
+      <c r="D21" s="74" t="s">
+        <v>78</v>
+      </c>
+      <c r="E21" s="75"/>
+      <c r="F21" s="76"/>
       <c r="G21" s="7" t="s">
         <v>17</v>
       </c>
@@ -2088,7 +2170,7 @@
       <c r="I21" s="20" t="s">
         <v>34</v>
       </c>
-      <c r="J21" s="35"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="4:11" x14ac:dyDescent="0.25">
       <c r="H22" s="5"/>
@@ -2103,13 +2185,14 @@
       <c r="H25" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="D21:F21"/>
     <mergeCell ref="J5:J8"/>
     <mergeCell ref="J13:J14"/>
     <mergeCell ref="D16:F16"/>
+    <mergeCell ref="J10:J11"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -2121,10 +2204,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B841B1-BE16-4D0F-8CFB-0CA1439E50F0}">
-  <dimension ref="D13:N26"/>
+  <dimension ref="D12:N26"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2135,187 +2218,192 @@
     <col min="14" max="14" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="12" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="87" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I13" s="98" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D14" s="63" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="84" t="s">
+        <v>75</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="I14" s="99" t="s">
+        <v>42</v>
+      </c>
+      <c r="J14" s="95" t="s">
+        <v>65</v>
+      </c>
+      <c r="K14" s="48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
+      <c r="D15" s="64"/>
+      <c r="E15" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="F13" s="32" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="50" t="s">
+      <c r="G15" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I15" s="99" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="96" t="s">
+        <v>65</v>
+      </c>
+      <c r="K15" s="49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D16" s="65"/>
+      <c r="E16" s="86" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I16" s="100" t="s">
         <v>59</v>
       </c>
-      <c r="I13" s="53" t="s">
+      <c r="J16" s="97"/>
+      <c r="K16" s="51"/>
+    </row>
+    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="E17" s="88" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="91" t="s">
+        <v>40</v>
+      </c>
+      <c r="G17" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="93" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="G14" s="50" t="s">
-        <v>58</v>
-      </c>
-      <c r="I14" s="52" t="s">
+      <c r="J17" s="96" t="s">
+        <v>65</v>
+      </c>
+      <c r="K17" s="49" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E18" s="89" t="s">
+        <v>74</v>
+      </c>
+      <c r="F18" s="92" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="64" t="s">
+      <c r="G18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="I18" s="99" t="s">
+        <v>60</v>
+      </c>
+      <c r="J18" s="96" t="s">
+        <v>65</v>
+      </c>
+      <c r="K18" s="49" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D19" s="80" t="s">
+        <v>78</v>
+      </c>
+      <c r="E19" s="81"/>
+      <c r="F19" s="81"/>
+      <c r="G19" s="93" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="J19" s="103"/>
+      <c r="K19" s="104"/>
+      <c r="L19" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="M19" s="23"/>
+    </row>
+    <row r="20" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D20" s="82" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="83"/>
+      <c r="F20" s="83"/>
+      <c r="G20" s="94" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="102" t="s">
+        <v>62</v>
+      </c>
+      <c r="J20" s="96" t="s">
+        <v>65</v>
+      </c>
+      <c r="K20" s="52" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J21" s="50"/>
+      <c r="K21" s="51"/>
+    </row>
+    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J22" s="50"/>
+      <c r="K22" s="51"/>
+    </row>
+    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J23" s="50"/>
+      <c r="K23" s="51"/>
+    </row>
+    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J24" s="50"/>
+      <c r="K24" s="51"/>
+    </row>
+    <row r="25" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J25" s="50"/>
+      <c r="K25" s="51"/>
+    </row>
+    <row r="26" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I26" s="101" t="s">
+        <v>35</v>
+      </c>
+      <c r="J26" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="K14" s="65" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="88"/>
-      <c r="E15" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="G15" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="I15" s="52" t="s">
-        <v>40</v>
-      </c>
-      <c r="J15" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="K15" s="67" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="89"/>
-      <c r="E16" s="29" t="s">
-        <v>73</v>
-      </c>
-      <c r="G16" s="50" t="s">
-        <v>56</v>
-      </c>
-      <c r="I16" s="60" t="s">
-        <v>60</v>
-      </c>
-      <c r="J16" s="68"/>
-      <c r="K16" s="69"/>
-    </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E17" s="58" t="s">
-        <v>74</v>
-      </c>
-      <c r="F17" s="54" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" s="50" t="s">
-        <v>55</v>
-      </c>
-      <c r="I17" s="61" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="K17" s="67" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="57" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="55" t="s">
-        <v>42</v>
-      </c>
-      <c r="G18" s="50" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="52" t="s">
-        <v>61</v>
-      </c>
-      <c r="J18" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="K18" s="67" t="s">
+      <c r="K26" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="L26" s="47" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="19" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D19" s="48"/>
-      <c r="E19" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="F19" s="48"/>
-      <c r="G19" s="53" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" s="50" t="s">
-        <v>62</v>
-      </c>
-      <c r="J19" s="70"/>
-      <c r="K19" s="71"/>
-      <c r="L19" s="23"/>
-      <c r="M19" s="23"/>
-    </row>
-    <row r="20" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="D20" s="48"/>
-      <c r="E20" s="48" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="48"/>
-      <c r="G20" s="49" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="62" t="s">
-        <v>63</v>
-      </c>
-      <c r="J20" s="66" t="s">
-        <v>66</v>
-      </c>
-      <c r="K20" s="72" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="J21" s="68"/>
-      <c r="K21" s="69"/>
-    </row>
-    <row r="22" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="J22" s="68"/>
-      <c r="K22" s="69"/>
-    </row>
-    <row r="23" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="J23" s="68"/>
-      <c r="K23" s="69"/>
-    </row>
-    <row r="24" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="J24" s="68"/>
-      <c r="K24" s="69"/>
-    </row>
-    <row r="25" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="J25" s="68"/>
-      <c r="K25" s="69"/>
-    </row>
-    <row r="26" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I26" s="63" t="s">
-        <v>35</v>
-      </c>
-      <c r="J26" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="K26" s="74" t="s">
-        <v>68</v>
-      </c>
-      <c r="L26" s="51" t="s">
-        <v>65</v>
-      </c>
-      <c r="M26" s="51"/>
-      <c r="N26" s="51"/>
+      <c r="M26" s="47"/>
+      <c r="N26" s="47"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="3">
     <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D19:F19"/>
+    <mergeCell ref="D20:F20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
added ESP32-CAM interrupt pin to pin-layout
</commit_message>
<xml_diff>
--- a/electronics/SpotMicroESP32_Pinout_v1_1_0_with_ESP32_CAM.xlsx
+++ b/electronics/SpotMicroESP32_Pinout_v1_1_0_with_ESP32_CAM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kubin\Projekte\SpotMicroESP32\electronics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44DFB44-748B-4617-A368-6AA01AE0E1FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2592F59C-31E4-4804-A820-1911DADEDBA2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{F9FC6447-11F2-4062-BA4B-EAD886E6EF95}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{F9FC6447-11F2-4062-BA4B-EAD886E6EF95}"/>
   </bookViews>
   <sheets>
     <sheet name="ESP32 DevKitC Connections" sheetId="2" r:id="rId1"/>
@@ -432,7 +432,7 @@
     <t>I2C Data</t>
   </si>
   <si>
-    <t>unassigned</t>
+    <t>RTC Interrupt</t>
   </si>
 </sst>
 </file>
@@ -553,7 +553,7 @@
       <family val="3"/>
     </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -702,6 +702,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1017,7 +1023,7 @@
     <xf numFmtId="0" fontId="12" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="105">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1"/>
@@ -1114,39 +1120,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1158,34 +1131,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="25" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1193,8 +1139,6 @@
     <xf numFmtId="0" fontId="0" fillId="13" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="12" fillId="23" borderId="20" xfId="5" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="21" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="17" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1206,7 +1150,67 @@
     <xf numFmtId="0" fontId="10" fillId="10" borderId="1" xfId="3" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="10" xfId="6" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Ausgabe" xfId="5" builtinId="21"/>
@@ -1317,7 +1321,7 @@
       <xdr:col>7</xdr:col>
       <xdr:colOff>3546528</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1845,7 +1849,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0F28E75-B5FB-4F1B-BA29-59D7A6CA9554}">
   <dimension ref="D1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3:F3"/>
     </sheetView>
   </sheetViews>
@@ -1864,11 +1868,11 @@
       <c r="H2" s="4"/>
     </row>
     <row r="3" spans="4:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D3" s="66" t="s">
+      <c r="D3" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="67"/>
-      <c r="F3" s="68"/>
+      <c r="E3" s="83"/>
+      <c r="F3" s="84"/>
       <c r="G3" s="7" t="s">
         <v>0</v>
       </c>
@@ -1876,11 +1880,11 @@
       <c r="I3" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="J3" s="66" t="s">
+      <c r="J3" s="82" t="s">
         <v>77</v>
       </c>
-      <c r="K3" s="67"/>
-      <c r="L3" s="68"/>
+      <c r="K3" s="83"/>
+      <c r="L3" s="84"/>
     </row>
     <row r="4" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="F4" s="34"/>
@@ -1896,10 +1900,10 @@
       <c r="L4" s="57"/>
     </row>
     <row r="5" spans="4:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E5" s="73" t="s">
+      <c r="E5" s="62" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="70" t="s">
+      <c r="F5" s="59" t="s">
         <v>81</v>
       </c>
       <c r="G5" s="9" t="s">
@@ -1909,21 +1913,21 @@
       <c r="I5" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="88" t="s">
         <v>36</v>
       </c>
       <c r="K5" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="L5" s="69" t="s">
+      <c r="L5" s="58" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="6" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E6" s="72" t="s">
+      <c r="E6" s="61" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="71" t="s">
+      <c r="F6" s="60" t="s">
         <v>83</v>
       </c>
       <c r="G6" s="10" t="s">
@@ -1933,7 +1937,7 @@
       <c r="I6" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="J6" s="59"/>
+      <c r="J6" s="89"/>
       <c r="K6" s="30"/>
     </row>
     <row r="7" spans="4:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1950,7 +1954,7 @@
       <c r="I7" s="27" t="s">
         <v>21</v>
       </c>
-      <c r="J7" s="59"/>
+      <c r="J7" s="89"/>
       <c r="K7" s="31"/>
     </row>
     <row r="8" spans="4:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.35">
@@ -1967,11 +1971,11 @@
       <c r="I8" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="J8" s="60"/>
+      <c r="J8" s="90"/>
       <c r="K8" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="L8" s="69" t="s">
+      <c r="L8" s="58" t="s">
         <v>80</v>
       </c>
     </row>
@@ -2010,10 +2014,10 @@
       <c r="I10" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="77" t="s">
+      <c r="J10" s="93" t="s">
         <v>85</v>
       </c>
-      <c r="K10" s="79" t="s">
+      <c r="K10" s="63" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2032,8 +2036,8 @@
       <c r="I11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="78"/>
-      <c r="K11" s="79" t="s">
+      <c r="J11" s="94"/>
+      <c r="K11" s="63" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2063,7 +2067,7 @@
       <c r="I13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="61" t="s">
+      <c r="J13" s="91" t="s">
         <v>41</v>
       </c>
       <c r="K13" s="32" t="s">
@@ -2079,7 +2083,7 @@
       <c r="I14" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="62"/>
+      <c r="J14" s="92"/>
       <c r="K14" s="33" t="s">
         <v>42</v>
       </c>
@@ -2096,11 +2100,11 @@
       <c r="J15" s="55"/>
     </row>
     <row r="16" spans="4:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="74" t="s">
+      <c r="D16" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="E16" s="75"/>
-      <c r="F16" s="76"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="87"/>
       <c r="G16" s="24" t="s">
         <v>1</v>
       </c>
@@ -2158,11 +2162,11 @@
       <c r="J20" s="34"/>
     </row>
     <row r="21" spans="4:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D21" s="74" t="s">
+      <c r="D21" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="75"/>
-      <c r="F21" s="76"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="87"/>
       <c r="G21" s="7" t="s">
         <v>17</v>
       </c>
@@ -2206,12 +2210,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33B841B1-BE16-4D0F-8CFB-0CA1439E50F0}">
   <dimension ref="D12:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" customWidth="1"/>
     <col min="7" max="7" width="11" customWidth="1"/>
     <col min="8" max="8" width="54.28515625" customWidth="1"/>
     <col min="9" max="9" width="12.42578125" customWidth="1"/>
@@ -2220,33 +2226,33 @@
   <sheetData>
     <row r="12" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E13" s="87" t="s">
+      <c r="E13" s="67" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="90" t="s">
+      <c r="F13" s="70" t="s">
         <v>69</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="I13" s="98" t="s">
+      <c r="I13" s="76" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D14" s="63" t="s">
+      <c r="D14" s="95" t="s">
         <v>76</v>
       </c>
-      <c r="E14" s="84" t="s">
+      <c r="E14" s="64" t="s">
         <v>75</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I14" s="99" t="s">
+      <c r="I14" s="77" t="s">
         <v>42</v>
       </c>
-      <c r="J14" s="95" t="s">
+      <c r="J14" s="73" t="s">
         <v>65</v>
       </c>
       <c r="K14" s="48" t="s">
@@ -2254,17 +2260,17 @@
       </c>
     </row>
     <row r="15" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="D15" s="64"/>
-      <c r="E15" s="85" t="s">
+      <c r="D15" s="96"/>
+      <c r="E15" s="65" t="s">
         <v>71</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="I15" s="99" t="s">
+      <c r="I15" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="J15" s="96" t="s">
+      <c r="J15" s="74" t="s">
         <v>65</v>
       </c>
       <c r="K15" s="49" t="s">
@@ -2272,33 +2278,33 @@
       </c>
     </row>
     <row r="16" spans="4:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D16" s="65"/>
-      <c r="E16" s="86" t="s">
+      <c r="D16" s="97"/>
+      <c r="E16" s="66" t="s">
         <v>72</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I16" s="100" t="s">
+      <c r="I16" s="78" t="s">
         <v>59</v>
       </c>
-      <c r="J16" s="97"/>
+      <c r="J16" s="75"/>
       <c r="K16" s="51"/>
     </row>
-    <row r="17" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="E17" s="88" t="s">
+    <row r="17" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="68" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="91" t="s">
+      <c r="F17" s="36" t="s">
         <v>40</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I17" s="93" t="s">
+      <c r="I17" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="J17" s="96" t="s">
+      <c r="J17" s="74" t="s">
         <v>65</v>
       </c>
       <c r="K17" s="49" t="s">
@@ -2306,19 +2312,19 @@
       </c>
     </row>
     <row r="18" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E18" s="89" t="s">
+      <c r="E18" s="69" t="s">
         <v>74</v>
       </c>
-      <c r="F18" s="92" t="s">
-        <v>42</v>
+      <c r="F18" s="102" t="s">
+        <v>88</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="I18" s="99" t="s">
+      <c r="I18" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="J18" s="96" t="s">
+      <c r="J18" s="74" t="s">
         <v>65</v>
       </c>
       <c r="K18" s="49" t="s">
@@ -2326,37 +2332,37 @@
       </c>
     </row>
     <row r="19" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D19" s="80" t="s">
+      <c r="D19" s="98" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="81"/>
-      <c r="F19" s="81"/>
-      <c r="G19" s="93" t="s">
+      <c r="E19" s="99"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="71" t="s">
         <v>1</v>
       </c>
       <c r="I19" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="J19" s="103"/>
-      <c r="K19" s="104"/>
-      <c r="L19" s="18" t="s">
-        <v>88</v>
-      </c>
+      <c r="J19" s="36" t="s">
+        <v>42</v>
+      </c>
+      <c r="K19" s="81"/>
+      <c r="L19" s="75"/>
       <c r="M19" s="23"/>
     </row>
     <row r="20" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D20" s="82" t="s">
+      <c r="D20" s="100" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="83"/>
-      <c r="F20" s="83"/>
-      <c r="G20" s="94" t="s">
+      <c r="E20" s="101"/>
+      <c r="F20" s="101"/>
+      <c r="G20" s="72" t="s">
         <v>17</v>
       </c>
-      <c r="I20" s="102" t="s">
+      <c r="I20" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="J20" s="96" t="s">
+      <c r="J20" s="74" t="s">
         <v>65</v>
       </c>
       <c r="K20" s="52" t="s">
@@ -2384,7 +2390,7 @@
       <c r="K25" s="51"/>
     </row>
     <row r="26" spans="4:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="I26" s="101" t="s">
+      <c r="I26" s="79" t="s">
         <v>35</v>
       </c>
       <c r="J26" s="53" t="s">

</xml_diff>